<commit_message>
finished a lot of model analysis, wrote functions
</commit_message>
<xml_diff>
--- a/supplemental/supplemental table 2.xlsx
+++ b/supplemental/supplemental table 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="-80" windowWidth="21360" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="-24460" yWindow="-520" windowWidth="21360" windowHeight="13520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>Highest Level Classification</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>%IncMSE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Top 15 in Spearman</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -138,22 +134,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Blautia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Otu00283</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>98-Blautia faecis</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Firmicutes</t>
   </si>
   <si>
@@ -224,6 +204,30 @@
   </si>
   <si>
     <t>Otu00064</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bacteroidetes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Otu00053</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Firmicutes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lachnospiraceae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>%IncMSE.filter.filter</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -231,11 +235,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -276,10 +281,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,14 +619,14 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -637,305 +644,299 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>6.2907397465560004</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>22.259889358755402</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
       <c r="G2">
-        <v>-0.70057803299999999</v>
+        <v>-0.63126108299999995</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3">
+        <v>40.973968335015201</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>13.440386405957399</v>
-      </c>
       <c r="G3">
-        <v>-0.51319346799999999</v>
+        <v>-0.80252450799999997</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3">
+        <v>21.2646478139796</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>18.457609759674</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
       <c r="G4">
-        <v>-0.78142163899999995</v>
+        <v>-0.76131644099999995</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5">
-        <v>2.2251158302826299</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3">
+        <v>39.791250132542103</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>0.335245079</v>
+        <v>-0.77247061800000005</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>41.772934132791697</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="3">
+        <v>14.783075179484101</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>-0.80252450799999997</v>
+        <v>0.56194013899999995</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3">
+        <v>23.5573073454716</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
-        <v>21.1561159901769</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
       <c r="G7">
-        <v>-0.76131644099999995</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>26</v>
+        <v>-0.72523814200000003</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3">
+        <v>39.845742491287901</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>-0.76214799799999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="4">
+        <v>13.946379759843801</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>-0.62844027499999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3">
+        <v>13.072308669846</v>
+      </c>
+      <c r="G10">
+        <v>-0.51319346799999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3">
+        <v>18.9413257929459</v>
+      </c>
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
-        <v>40.008732327557603</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8">
-        <v>-0.77247061800000005</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="G11">
+        <v>-0.78142163899999995</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3">
+        <v>15.8299461388319</v>
+      </c>
+      <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>23.483418302741601</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9">
-        <v>-0.72523814200000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>38.012390790312502</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10">
-        <v>-0.76214799799999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11">
-        <v>5.8790654311659702</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>-0.63126108299999995</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>15.266990651110699</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
       <c r="G12">
-        <v>0.145581395873738</v>
-      </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
-        <v>36</v>
+        <v>-0.72941687399999999</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>31.2360831271974</v>
+        <v>11</v>
+      </c>
+      <c r="E13" s="3">
+        <v>32.3272101581627</v>
       </c>
       <c r="G13">
         <v>-0.62451203200000005</v>
@@ -943,207 +944,206 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3">
+        <v>23.7322154842687</v>
+      </c>
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="E14">
-        <v>20.867613085964699</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
       <c r="G14">
-        <v>-0.76919188199999999</v>
-      </c>
-      <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
+        <v>-0.70057803299999999</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3">
+        <v>20.4642382408421</v>
+      </c>
+      <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="E15">
-        <v>15.607993981976399</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
       <c r="G15">
-        <v>-0.72941687399999999</v>
+        <v>-0.76919188199999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>11.8683218490602</v>
+        <v>20</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="3">
+        <v>3.2033162786076401</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
       </c>
       <c r="G16">
-        <v>-0.468791202360753</v>
+        <v>0.335245079</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17">
-        <v>19.156643550432101</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="3">
+        <v>11.9571411161299</v>
       </c>
       <c r="G17">
-        <v>0.36237248999999999</v>
+        <v>-0.42739072790824001</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>15.410392937770499</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18">
-        <v>0.56194013899999995</v>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="4">
+        <v>18.524701731201301</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>-0.58309034800000004</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19">
-        <v>5.8962860550684901</v>
+      <c r="E19" s="3">
+        <v>7.4081701925228201</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19">
         <v>0.31451523599999998</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3">
+        <v>21.2738551886893</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <v>0.36237248999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20">
-        <v>4.5869095609408799</v>
-      </c>
-      <c r="F20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20">
+      <c r="E21" s="3">
+        <v>5.7926565021299599</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
         <v>0.31292503599999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="2">
-        <v>14.894766900322701</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <v>-0.62844027499999999</v>
-      </c>
-    </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="2">
-        <v>18.532256119361499</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <v>-0.58309034800000004</v>
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="3">
+        <v>15.6627763224954</v>
+      </c>
+      <c r="G22">
+        <v>-0.468791202360753</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
+  <sortState ref="A2:XFD22">
+    <sortCondition ref="A3:A22"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
cont'd work on model revisions
</commit_message>
<xml_diff>
--- a/supplemental/supplemental table 2.xlsx
+++ b/supplemental/supplemental table 2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="21040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="-16680" yWindow="2860" windowWidth="21040" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>Highest Level Classification</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -229,6 +229,69 @@
   <si>
     <t>%IncMSE.filter.filter</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Otu00004</t>
+  </si>
+  <si>
+    <t>Otu00097</t>
+  </si>
+  <si>
+    <t>Otu00073</t>
+  </si>
+  <si>
+    <t>Otu00042</t>
+  </si>
+  <si>
+    <t>Otu00005</t>
+  </si>
+  <si>
+    <t>Otu00010</t>
+  </si>
+  <si>
+    <t>Otu00014</t>
+  </si>
+  <si>
+    <t>Otu00092</t>
+  </si>
+  <si>
+    <t>Otu00001</t>
+  </si>
+  <si>
+    <t>Otu00081</t>
+  </si>
+  <si>
+    <t>Otu00086</t>
+  </si>
+  <si>
+    <t>Ruminococcus</t>
+  </si>
+  <si>
+    <t>Otu00026</t>
+  </si>
+  <si>
+    <t>Otu00018</t>
+  </si>
+  <si>
+    <t>Otu00038</t>
+  </si>
+  <si>
+    <t>Ruminococcaceae</t>
+  </si>
+  <si>
+    <t>Otu00012</t>
+  </si>
+  <si>
+    <t>Otu00033</t>
+  </si>
+  <si>
+    <t>Otu00009</t>
+  </si>
+  <si>
+    <t>Otu00050</t>
+  </si>
+  <si>
+    <t>Coriobacteriaceae</t>
   </si>
 </sst>
 </file>
@@ -280,12 +343,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1139,6 +1203,258 @@
         <v>0.335245079</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <v>12.603463963579401</v>
+      </c>
+      <c r="G25">
+        <v>-0.62048909673570196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26">
+        <v>12.2390926998055</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27">
+        <v>12.0270125031301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28">
+        <v>10.970855663631699</v>
+      </c>
+      <c r="G28">
+        <v>-0.54622065303771095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>10.7539928883744</v>
+      </c>
+      <c r="G29">
+        <v>-0.55658991312276895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30">
+        <v>10.590521026570499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31">
+        <v>10.504217422815501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32">
+        <v>10.3323152256946</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33">
+        <v>9.8008163847131193</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35">
+        <v>-0.61834182123088299</v>
+      </c>
+      <c r="H35" s="5">
+        <v>1.6606556005146901E-10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36">
+        <v>-0.58461145886863497</v>
+      </c>
+      <c r="H36" s="5">
+        <v>3.4072736120638401E-9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37">
+        <v>-0.57602798245480202</v>
+      </c>
+      <c r="H37" s="5">
+        <v>6.4435586788493901E-9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38">
+        <v>-0.560682964582215</v>
+      </c>
+      <c r="H38" s="5">
+        <v>2.09693698898655E-8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39">
+        <v>-0.55818769337937801</v>
+      </c>
+      <c r="H39" s="5">
+        <v>2.4530082470993301E-8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40">
+        <v>-0.55172532091891902</v>
+      </c>
+      <c r="H40" s="5">
+        <v>3.7719492985284103E-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41">
+        <v>-0.53215242792609996</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1.5511480954107601E-7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>-0.50230339850246797</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1.1392277530317E-6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43">
+        <v>-0.50154276003387599</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1.1600624557794101E-6</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <sortState ref="A2:XFD22">
@@ -1146,6 +1462,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>